<commit_message>
Update Rizka - Update Object Cari Mobil Rental
</commit_message>
<xml_diff>
--- a/Logout.xlsx
+++ b/Logout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3E25A7-9311-4DE5-AA4E-39BA46E5781E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48B5D19-43E4-4F36-BFF2-075CD6931B8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{CBF1FAE6-460B-40EB-B596-EF8549460824}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="13440" windowHeight="11070" xr2:uid="{CBF1FAE6-460B-40EB-B596-EF8549460824}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>